<commit_message>
Change log: #70 aggregation script
#69 implementing hardware monitoring adding it to the experiment class

#62 adding to report frist draft for the report without evaluation part is done
</commit_message>
<xml_diff>
--- a/research_master/experiment_overview.xlsx
+++ b/research_master/experiment_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\PyMatch\research_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6187E7EA-3BB0-4EE5-9224-E54DC79C5A0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25CD339-EC76-4802-86B4-494D536D0D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17040" yWindow="690" windowWidth="14115" windowHeight="12345" xr2:uid="{2DDCFFEB-27E5-4D64-9567-EDADF09471CE}"/>
+    <workbookView xWindow="-20115" yWindow="1890" windowWidth="14115" windowHeight="12345" xr2:uid="{2DDCFFEB-27E5-4D64-9567-EDADF09471CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="158">
   <si>
     <t>Experiment</t>
   </si>
@@ -411,6 +411,110 @@
   </si>
   <si>
     <t>like 58 but smaller lr</t>
+  </si>
+  <si>
+    <t>20 identical experiments
+used for evaluation for report
+it uses the same dropout as the MC evaluation and should therefore be comparable</t>
+  </si>
+  <si>
+    <t>Series of 10 experiments</t>
+  </si>
+  <si>
+    <t>exp_76</t>
+  </si>
+  <si>
+    <t>exp_77</t>
+  </si>
+  <si>
+    <t>exp_78</t>
+  </si>
+  <si>
+    <t>exp_79</t>
+  </si>
+  <si>
+    <t>exp_80</t>
+  </si>
+  <si>
+    <t>exp_81</t>
+  </si>
+  <si>
+    <t>exp_82</t>
+  </si>
+  <si>
+    <t>exp_83</t>
+  </si>
+  <si>
+    <t>exp_84</t>
+  </si>
+  <si>
+    <t>exp_85</t>
+  </si>
+  <si>
+    <t>exp_86</t>
+  </si>
+  <si>
+    <t>exp_87</t>
+  </si>
+  <si>
+    <t>exp_88</t>
+  </si>
+  <si>
+    <t>exp_89</t>
+  </si>
+  <si>
+    <t>exp_90</t>
+  </si>
+  <si>
+    <t>exp_91</t>
+  </si>
+  <si>
+    <t>exp_92</t>
+  </si>
+  <si>
+    <t>exp_93</t>
+  </si>
+  <si>
+    <t>exp_94</t>
+  </si>
+  <si>
+    <t>exp_95</t>
+  </si>
+  <si>
+    <t>exp_96</t>
+  </si>
+  <si>
+    <t>exp_97</t>
+  </si>
+  <si>
+    <t>exp_98</t>
+  </si>
+  <si>
+    <t>exp_99</t>
+  </si>
+  <si>
+    <t>exp_100</t>
+  </si>
+  <si>
+    <t>exp_101</t>
+  </si>
+  <si>
+    <t>exp_102</t>
+  </si>
+  <si>
+    <t>exp_103</t>
+  </si>
+  <si>
+    <t>exp_104</t>
+  </si>
+  <si>
+    <t>exp_105</t>
+  </si>
+  <si>
+    <t>exp_106</t>
+  </si>
+  <si>
+    <t>exp_107</t>
   </si>
 </sst>
 </file>
@@ -779,17 +883,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F221E8-4732-4970-8978-EF44361568AC}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1905,25 +2009,236 @@
       <c r="A72" t="s">
         <v>82</v>
       </c>
+      <c r="B72" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" t="s">
+        <v>48</v>
+      </c>
+      <c r="D73" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>84</v>
+      </c>
+      <c r="B74" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>85</v>
       </c>
+      <c r="B75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" t="s">
+        <v>45</v>
+      </c>
+      <c r="D75" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>86</v>
+      </c>
+      <c r="B76" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" t="s">
+        <v>45</v>
+      </c>
+      <c r="D76" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>